<commit_message>
End Year 1 Probation
</commit_message>
<xml_diff>
--- a/Manual_DataMining_Microsrvc_Apps.xlsx
+++ b/Manual_DataMining_Microsrvc_Apps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gleschen/Documents/PhD research UoL/uol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4658215-508E-C242-9E7D-861B8E4AA3CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C569759-6CAC-524C-9743-3957100FE8CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14720" xr2:uid="{0F28AD2F-1EE6-CF4C-BEE4-2E79DDB61BE6}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="231">
-  <si>
-    <t>Docker host</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="248">
   <si>
     <t>Web App MVC</t>
   </si>
@@ -73,13 +69,6 @@
     <t xml:space="preserve">Frontend </t>
   </si>
   <si>
-    <t>Go
-NodeJs
-Python
-C#
-Java</t>
-  </si>
-  <si>
     <t>Communication Protocol</t>
   </si>
   <si>
@@ -87,11 +76,6 @@
   </si>
   <si>
     <t>Eureka</t>
-  </si>
-  <si>
-    <t>HTTP
-RESTful
-JPA/SQL</t>
   </si>
   <si>
     <t>Chrome
@@ -110,12 +94,6 @@
     <t>Spring Boot</t>
   </si>
   <si>
-    <t xml:space="preserve">HTTP
-REST
-gRPC
-</t>
-  </si>
-  <si>
     <t>Docker host
 Docker compose
 Kubernetes
@@ -158,11 +136,6 @@
   <si>
     <t>Docker
 Kubernetes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Python
-Nodejs
-</t>
   </si>
   <si>
     <t>MySQL</t>
@@ -849,21 +822,6 @@
 MongoDB</t>
   </si>
   <si>
-    <t>SQL Server DB
-MongoDB
-CosmosDB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aggregator Microservices (Envoy, istio GW, C# graphql)
-Domain Microservices </t>
-  </si>
-  <si>
-    <t>MongoDB 
-MySQL 
-Redis
-NEST (ElasticSearch)</t>
-  </si>
-  <si>
     <t>MySQL
 MongoDB
 Redis</t>
@@ -907,6 +865,161 @@
   <si>
     <t>DB2
 MongoDB</t>
+  </si>
+  <si>
+    <t>Identity
+Catalog
+ordering
+Basket
+Marketing
+Locations</t>
+  </si>
+  <si>
+    <t>SQL Server 
+SQL Server 
+SQL Server
+Redis Cache
+MongoDB/CosmosDB/SQL Server
+MongoDB/CosmosDB</t>
+  </si>
+  <si>
+    <t>Frontend
+Cart
+Recommendation
+ProductCatalog
+Currency
+Shipping
+Checkout
+Payment
+Email
+Ad</t>
+  </si>
+  <si>
+    <t>Go
+C#
+Go
+NodeJs
+NodeJs
+Go
+Python
+Go
+Python
+Java</t>
+  </si>
+  <si>
+    <t>Docker
+Azure</t>
+  </si>
+  <si>
+    <t>Registration (Eureka)
+Account 
+Web</t>
+  </si>
+  <si>
+    <t>RESTful
+JPA/SQL</t>
+  </si>
+  <si>
+    <t>Aggregator microservices: 
+Envoy
+istio GW, 
+C# graphql
+Domain Microservices:
+Catalog
+Rating
+Cart
+Inventory</t>
+  </si>
+  <si>
+    <t>MongoDB 
+MongoDB
+MySQL 
+MySQL
+Redis
+NEST (ElasticSearch)</t>
+  </si>
+  <si>
+    <t>HTTP
+REST
+gRPC</t>
+  </si>
+  <si>
+    <t>Catalog
+Review
+Recommendation
+Order
+Customer
+Configuration
+Auth</t>
+  </si>
+  <si>
+    <t>Identity
+Transaction</t>
+  </si>
+  <si>
+    <t>Azure</t>
+  </si>
+  <si>
+    <t>Transaction
+Compute Interest
+Notification</t>
+  </si>
+  <si>
+    <t>Python
+Nodejs</t>
+  </si>
+  <si>
+    <t>Service-one
+Service-two
+Service-three</t>
+  </si>
+  <si>
+    <t>MySQL
+MySQL
+MySQL</t>
+  </si>
+  <si>
+    <t>RabbitMQ
+RabbitMQ
+RabbitMQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consul </t>
+  </si>
+  <si>
+    <t>Drivers
+Trips
+Trip Manager &amp; Monitor
+Passengers</t>
+  </si>
+  <si>
+    <t>MS SQL
+MongoDB</t>
+  </si>
+  <si>
+    <t>Authorization
+Order
+Customer
+Inventory
+Product
+Shipping</t>
+  </si>
+  <si>
+    <t>Authentication and Autorisation
+Frontend
+Dashboard</t>
+  </si>
+  <si>
+    <t>Contact
+Communication
+Coming
+Identity</t>
+  </si>
+  <si>
+    <t>Player
+Auth
+Mediator
+Room</t>
   </si>
 </sst>
 </file>
@@ -957,7 +1070,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -980,11 +1093,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -993,6 +1158,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1309,8 +1482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC060CB0-B6EF-C345-B4A3-FB787C42CDE0}">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B87" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1318,8 +1491,8 @@
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.5" customWidth="1"/>
+    <col min="5" max="5" width="35.83203125" customWidth="1"/>
     <col min="6" max="6" width="28.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="24.5" bestFit="1" customWidth="1"/>
@@ -1330,86 +1503,88 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="85" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
+    <row r="3" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
+      <c r="D3" s="4" t="s">
+        <v>225</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>14</v>
+        <v>226</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -1417,376 +1592,384 @@
     <row r="4" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
+      <c r="D4" s="4" t="s">
+        <v>228</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="4" t="s">
-        <v>18</v>
+        <v>229</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>23</v>
+        <v>232</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>233</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>235</v>
+      </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>234</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>6</v>
+      <c r="D8" s="4" t="s">
+        <v>236</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="4" t="s">
-        <v>35</v>
+        <v>237</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>36</v>
+        <v>1</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>239</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>37</v>
+        <v>240</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>241</v>
+      </c>
       <c r="K9" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>221</v>
+        <v>38</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>213</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>6</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D11" s="9"/>
       <c r="E11" s="3"/>
       <c r="F11" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>245</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
-        <v>6</v>
+      <c r="C14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>6</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
-        <v>6</v>
+      <c r="D16" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -1794,187 +1977,187 @@
     </row>
     <row r="18" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="D24" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="51" x14ac:dyDescent="0.2">
@@ -1982,138 +2165,138 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
     </row>
     <row r="27" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -2123,217 +2306,217 @@
     </row>
     <row r="31" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
     </row>
     <row r="36" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J36" s="3"/>
       <c r="K36" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
     </row>
     <row r="38" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J38" s="3"/>
       <c r="K38" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
@@ -2341,46 +2524,46 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
@@ -2388,104 +2571,104 @@
     </row>
     <row r="42" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -2493,15 +2676,15 @@
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
@@ -2511,87 +2694,87 @@
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
     </row>
     <row r="48" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="J48" s="3"/>
       <c r="K48" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="K49" s="3"/>
     </row>
     <row r="50" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
@@ -2602,10 +2785,10 @@
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -2616,107 +2799,107 @@
     </row>
     <row r="52" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
     </row>
     <row r="53" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G53" s="3"/>
       <c r="H53" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J53" s="3"/>
       <c r="K53" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J54" s="3"/>
       <c r="K54" s="3" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K55" s="3"/>
     </row>
@@ -2725,103 +2908,103 @@
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I57" s="3"/>
       <c r="J57" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K57" s="3"/>
     </row>
     <row r="58" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
     </row>
     <row r="59" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -2829,7 +3012,7 @@
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
@@ -2841,25 +3024,25 @@
     </row>
     <row r="61" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
@@ -2867,52 +3050,52 @@
     <row r="62" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
       <c r="B62" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K62" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K63" s="3"/>
     </row>
@@ -2921,85 +3104,85 @@
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
       <c r="I64" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J64" s="3"/>
       <c r="K64" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K65" s="3"/>
     </row>
     <row r="66" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K66" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -3007,79 +3190,79 @@
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
       <c r="H68" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
     </row>
     <row r="69" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
       <c r="H69" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I69" s="3"/>
       <c r="J69" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K69" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
@@ -3087,68 +3270,68 @@
     </row>
     <row r="71" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K71" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="72" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
       <c r="J72" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K72" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
@@ -3156,22 +3339,22 @@
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
       <c r="J73" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K73" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
@@ -3180,7 +3363,7 @@
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
       <c r="K74" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -3188,45 +3371,45 @@
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="4" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G75" s="3"/>
       <c r="H75" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
       <c r="K75" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="76" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
@@ -3234,146 +3417,146 @@
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="3"/>
       <c r="B77" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E77" s="3"/>
       <c r="F77" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G77" s="3"/>
       <c r="H77" s="3" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="B78" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
       <c r="I78" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="I79" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J79" s="3"/>
       <c r="K79" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G80" s="3"/>
       <c r="H80" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="J80" s="3"/>
       <c r="K80" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G81" s="3"/>
       <c r="H81" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K81" s="3"/>
     </row>
     <row r="82" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
       <c r="H82" s="4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
@@ -3381,22 +3564,22 @@
     </row>
     <row r="83" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="G83" s="3"/>
       <c r="H83" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="I83" s="3"/>
       <c r="J83" s="3"/>
@@ -3406,56 +3589,56 @@
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="G84" s="3"/>
       <c r="H84" s="4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I84" s="3"/>
       <c r="J84" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K84" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="85" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
       <c r="J85" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K85" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="86" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -3463,36 +3646,36 @@
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E86" s="3"/>
       <c r="F86" s="4" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="G86" s="3"/>
       <c r="H86" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I86" s="3"/>
       <c r="J86" s="3"/>
       <c r="K86" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
@@ -3504,10 +3687,10 @@
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
@@ -3515,56 +3698,56 @@
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
       <c r="J88" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K88" s="3"/>
     </row>
     <row r="89" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="I89" s="3"/>
       <c r="J89" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K89" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D90" s="3"/>
       <c r="E90" s="4"/>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
       <c r="H90" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
       <c r="K90" s="3" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
@@ -3582,32 +3765,32 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
       <c r="E92" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
       <c r="E93" s="3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
@@ -3618,23 +3801,23 @@
     </row>
     <row r="94" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="G94" s="3"/>
       <c r="H94" s="4" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I94" s="4" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
@@ -3642,17 +3825,17 @@
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="3"/>
       <c r="B95" s="3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
       <c r="H95" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="I95" s="3"/>
       <c r="J95" s="3"/>
@@ -3660,22 +3843,22 @@
     </row>
     <row r="96" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
       <c r="H96" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I96" s="3"/>
       <c r="J96" s="3"/>
@@ -3683,25 +3866,25 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
       <c r="H97" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="I97" s="3"/>
       <c r="J97" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="K97" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
@@ -3709,11 +3892,11 @@
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
@@ -3723,43 +3906,43 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C99" s="3"/>
       <c r="D99" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
       <c r="I99" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
     </row>
     <row r="100" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F100" s="3"/>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
       <c r="J100" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K100" s="3"/>
     </row>

</xml_diff>